<commit_message>
Login e App Adm rodando
</commit_message>
<xml_diff>
--- a/banco_de_dados/BD.xlsx
+++ b/banco_de_dados/BD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="logins" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,8 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -49,7 +51,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -58,7 +60,9 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +443,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -511,7 +515,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>t-(00)90000-0000</t>
+          <t>(87)98888-8888</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -528,42 +532,43 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cli001</t>
+          <t>tec001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cli123</t>
+          <t>S@123</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>cpf-111.111.111-75</t>
+          <t>109.283.604-74</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>cliente Silva</t>
+          <t>Samuel Guilherme Borba Ramos</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>t-(00)90000-0001</t>
+          <t>(87)98814-8431</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>manhã</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>TI Team</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -573,30 +578,34 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
   <cols>
-    <col width="13.25" customWidth="1" min="1" max="1"/>
+    <col width="16.75" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="13.25" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="16.375" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13.25" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13.25" customWidth="1" min="5" max="5"/>
-    <col width="18.25" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="10.25" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="11.25" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="15.75" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="30.875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="16.875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="18.25" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="18.25" customWidth="1" min="8" max="8"/>
+    <col width="19.75" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="19.75" customWidth="1" min="10" max="10"/>
+    <col width="10.25" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="11.25" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="15.75" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="30.875" bestFit="1" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Código Peça</t>
+          <t>ID da ferramenta</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -606,59 +615,39 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Peça</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Situação</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Fabricante</t>
+          <t>Mensagem</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Situação</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Descrição</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Mensagem</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>Ação</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Ação: aquisição ou descarte</t>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Ação: compra ou descarte</t>
         </is>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ch_f0001</t>
+          <t>1-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -666,47 +655,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C2" t="n">
+        <v>35</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ch_f0002</t>
+          <t>1-0002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -714,47 +688,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C3" t="n">
+        <v>35</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ch_f0003</t>
+          <t>1-0003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -762,47 +721,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K4" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C4" t="n">
+        <v>35</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ch_f0004</t>
+          <t>1-0004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -810,47 +754,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C5" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ch_f0005</t>
+          <t>1-0005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -858,47 +787,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H6" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="n"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K6" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C6" t="n">
+        <v>35</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ch_f0006</t>
+          <t>1-0006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -906,47 +820,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="n"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ch_f0007</t>
+          <t>1-0007</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -954,47 +853,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K8" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C8" t="n">
+        <v>35</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>44885</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ch_f0008</t>
+          <t>2-0001</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1002,47 +886,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H9" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I9" s="3" t="n"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K9" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C9" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>44612</v>
       </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ch_f0009</t>
+          <t>2-0002</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1050,47 +919,32 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>140.8</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H10" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I10" s="3" t="n"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K10" s="4" t="n">
-        <v>44868.41666666666</v>
+      <c r="C10" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>44612</v>
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ch_f0010</t>
+          <t>2-0003</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1098,95 +952,953 @@
           <t>adm001</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>136.62</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I11" s="3" t="n"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>compra</t>
-        </is>
-      </c>
-      <c r="K11" s="4" t="n">
-        <v>44866.41666666666</v>
+      <c r="C11" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>44612</v>
       </c>
     </row>
     <row r="12" ht="16.5" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ch_f0001</t>
+          <t>2-0004</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>cli001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Chave de fenda</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Gedore</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>91891</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="H12" s="3" t="inlineStr">
-        <is>
-          <t>Fabricado em Aço Molibdênio-Vanadium-Plus e polímero anti-chamas, nas cores vermelho e amarelo, padrão Gedore. Haste com acabamento escurecido e revestimento produzido por injeção, propiciando isolação até 1000 V, conforme norma EN 60900 / IEC 60900, submetida à ensaios de: impacto, tensão elétrica, aderência, inflamabilidade, pressão/penetração. Empunhadura ergonômica em 3 componentes Power-Grip 3, que permite ao operador a execução do trabalho preciso e sem fadiga, devido ao ajuste positivo da empunhadura e lâmina para transmissão de força adequada. Encaixe identificado no final da empunhadura. Chave com haste redonda e resistente, com perfil de encaixe para parafuso tipo fenda simples.
-*ATENÇÃO: Utilizar ferramentas isoladas VDE, em tensão máxima de 1000 V em corrente alternada e 1500 V em corrente contínua, conforme norma EN 60900 / IEC 60900. Atende com segurança a norma regulamentadora NR 10 - Segurança em Instalações e Serviços em Eletricidade, possui certificado de isolação.</t>
-        </is>
-      </c>
-      <c r="I12" s="3" t="n"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Retirada</t>
-        </is>
-      </c>
-      <c r="K12" s="4" t="n">
-        <v>44868.5625</v>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>44612</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="H13" s="3" t="n"/>
-      <c r="I13" s="3" t="n"/>
-      <c r="K13" s="4" t="n"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2-0005</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>44612</v>
+      </c>
+      <c r="L13" s="3" t="n"/>
+      <c r="M13" s="3" t="n"/>
+      <c r="O13" s="4" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2-0006</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2-0007</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2-0008</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2-0009</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2-0010</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2-0011</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2-0012</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2-0013</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2-0014</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2-0015</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2-0016</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2-0017</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2-0018</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2-0019</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2-0020</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>165.8</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3-0001</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>328.3</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>44599</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>3-0002</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>328.3</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>44599</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>3-0003</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>328.3</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>44599</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>tec001</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>retirada</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>44890</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>tec001</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>devolução</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>44891</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>tec001</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>retirada</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>44893</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>tec001</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Defeito</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>borracha do cabo</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>devolução</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>44894</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Defeito</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Reparo no cabo</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>manutenção</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>44894</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1-0001</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>reparada</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>devolução</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2-0021</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G38" s="8" t="n">
+        <v>44683</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2-0022</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>adm001</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Nova</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>compra</t>
+        </is>
+      </c>
+      <c r="G39" s="8" t="n">
+        <v>44683</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1198,8 +1910,8 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="A12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -1211,10 +1923,10 @@
     <col width="62.125" customWidth="1" min="5" max="5"/>
     <col width="11.25" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="10.75" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="15.625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="26.875" customWidth="1" min="8" max="8"/>
     <col width="16.75" bestFit="1" customWidth="1" min="9" max="9"/>
     <col width="26.875" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="19.75" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="19.75" bestFit="1" customWidth="1" style="6" min="11" max="11"/>
     <col width="13.125" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -1269,7 +1981,7 @@
           <t>Data pedido/liberada reserva</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="6" t="inlineStr">
         <is>
           <t>tempo pedido/limite</t>
         </is>
@@ -1283,7 +1995,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cliente Silva_1</t>
+          <t>cli001_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1296,9 +2008,9 @@
           <t>pedido</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ch_f0001</t>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>1-0001</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1326,7 +2038,7 @@
         <v>44868.5625</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -1337,7 +2049,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cliente Silva_1</t>
+          <t>cli001_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1350,9 +2062,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ch_f0001</t>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>1-0001</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1374,14 +2086,14 @@
         <v>44867.41666666666</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>44867.47916666666</v>
+        <v>44867.48611111111</v>
       </c>
       <c r="J3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cliente Silva_1</t>
+          <t>cli001_1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1394,9 +2106,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ch_f0001</t>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>1-0001</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1418,13 +2130,13 @@
         <v>44867.41666666666</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>44867.5625</v>
+        <v>44867.57638888889</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cliente Silva_1</t>
+          <t>cli001_1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1437,9 +2149,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ch_f0001</t>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>1-0001</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1461,19 +2173,19 @@
         <v>44867.41666666666</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>44867.56944444445</v>
+        <v>44867.58333333334</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>44868.5625</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cliente Silva_2</t>
+          <t>cli001_2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1486,9 +2198,9 @@
           <t>pedido</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ch_f0002</t>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>1-0002</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1516,13 +2228,13 @@
         <v>44868.5625</v>
       </c>
       <c r="K6" s="6" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cliente Silva_2</t>
+          <t>cli001_2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1535,9 +2247,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ch_f0002</t>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>1-0002</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1566,7 +2278,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cliente Silva_2</t>
+          <t>cli001_2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1579,9 +2291,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ch_f0002</t>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>1-0002</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1609,7 +2321,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cliente Silva_2</t>
+          <t>cli001_2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1622,9 +2334,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ch_f0002</t>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>1-0002</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1652,13 +2364,13 @@
         <v>44868.5625</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cliente Silva_3</t>
+          <t>cli001_3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1671,9 +2383,9 @@
           <t>pedido</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ch_f0003</t>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>1-0003</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1701,13 +2413,13 @@
         <v>44868.5625</v>
       </c>
       <c r="K10" s="6" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cliente Silva_3</t>
+          <t>cli001_3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1720,9 +2432,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ch_f0003</t>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>1-0003</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1751,7 +2463,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cliente Silva_3</t>
+          <t>cli001_3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1764,9 +2476,9 @@
           <t>resposta</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ch_f0003</t>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>1-0003</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1792,10 +2504,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="H13" s="5" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="6" t="n"/>
+      <c r="H13" s="7" t="n"/>
+      <c r="I13" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
@@ -1809,26 +2519,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
   <cols>
     <col width="15.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="17.125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="14.875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.75" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="22.375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="24.375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="24.375" customWidth="1" min="4" max="4"/>
+    <col width="16.625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="16.625" customWidth="1" min="6" max="6"/>
+    <col width="9.125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="19.5" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="19.5" customWidth="1" min="9" max="9"/>
+    <col width="22.375" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="27.25" bestFit="1" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>codigo primario</t>
+          <t>ID da ferramenta</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1838,29 +2553,54 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>uso ferramenta</t>
+          <t>Descrição da ferramenta</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>voltagem</t>
+          <t xml:space="preserve">Fabricante  </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>tamanho</t>
+          <t>Voltagem de uso</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>material da ferramenta</t>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tamanho  </t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Unidade de medida</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Tipo de ferramenta</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Material da ferramenta</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Tempo de reserva esperado</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ch_f</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1870,26 +2610,200 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">desafrochar </t>
+          <t>Cruzada Isolada</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Gedore</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10 mm</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>91800</v>
+      </c>
+      <c r="G2" t="n">
+        <v>150</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Chave de fenda</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Aço</t>
         </is>
       </c>
-    </row>
+      <c r="K2" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kit epi contrução civil</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kit completo</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Santana</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1560515</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>sem medida</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>EPI</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>s/n</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Furadeira de Impacto 1/2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23 acessórios</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Skil</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>6555</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>cm</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Furadeira</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Aço</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>T s6 lite</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>110-220</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>891891</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Polegadas</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>multiplos</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>